<commit_message>
Mejoras en las importacion de ChromeDriver
</commit_message>
<xml_diff>
--- a/cargadetlectiva-masivo.xlsx
+++ b/cargadetlectiva-masivo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\acarganolectiva\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gians\Desktop\dev\UNDC_AUTOMATIZACION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99B17C5-73EE-47D5-ACE5-E0631B0CD20B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D793E92-A59E-4713-889B-84C5BE1CD516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{AC3D8E4D-96C0-40C7-9193-949C63F87DF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AC3D8E4D-96C0-40C7-9193-949C63F87DF0}"/>
   </bookViews>
   <sheets>
     <sheet name="cargas" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="90">
   <si>
     <t>HORAE</t>
   </si>
@@ -273,20 +273,50 @@
     <t>QUITAR</t>
   </si>
   <si>
-    <t>CONSULTAR SI SE VA A CREAR DESDE LA SEM 1</t>
-  </si>
-  <si>
-    <t>REVISAR SI ESTA BIEN SU CARGA LECTIVA DE PRACTICA</t>
-  </si>
-  <si>
     <t>OBS</t>
+  </si>
+  <si>
+    <t>BOTÁNICA GENERAL</t>
+  </si>
+  <si>
+    <t>VEGA RONQUILLO MANUEL</t>
+  </si>
+  <si>
+    <t>https://sivireno.undc.edu.pe/index_home.php?s=asistencia_cursos.php&amp;id_dcl=25</t>
+  </si>
+  <si>
+    <t>https://sivireno.undc.edu.pe/index_home.php?s=asistencia_cursos.php&amp;id_dcl=26</t>
+  </si>
+  <si>
+    <t>FERTILIDAD DEL SUELO</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>https://sivireno.undc.edu.pe/index_home.php?s=asistencia_cursos.php&amp;id_dcl=27</t>
+  </si>
+  <si>
+    <t>https://sivireno.undc.edu.pe/index_home.php?s=asistencia_cursos.php&amp;id_dcl=28</t>
+  </si>
+  <si>
+    <t>HORASREGISTRADAS</t>
+  </si>
+  <si>
+    <t>6-16</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +346,13 @@
       <name val="Source Sans Pro"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -326,7 +363,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -359,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -368,9 +405,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -957,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2442F8-A25A-4C8B-994C-1CDF0A0D4BA8}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,6 +1015,7 @@
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="9" width="6.28515625" customWidth="1"/>
     <col min="11" max="12" width="6.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1013,8 +1055,11 @@
       <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
-        <v>79</v>
+      <c r="M1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1039,12 +1084,6 @@
       <c r="G2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-      <c r="I2">
-        <v>16</v>
-      </c>
       <c r="J2" t="s">
         <v>13</v>
       </c>
@@ -1053,6 +1092,9 @@
       </c>
       <c r="L2" s="2">
         <v>0.5</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="O2" s="5"/>
     </row>
@@ -1078,12 +1120,6 @@
       <c r="G3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H3">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>16</v>
-      </c>
       <c r="J3" t="s">
         <v>11</v>
       </c>
@@ -1093,50 +1129,46 @@
       <c r="L3" s="2">
         <v>0.53125</v>
       </c>
-      <c r="M3" t="s">
-        <v>77</v>
+      <c r="M3" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="6">
-        <v>6</v>
-      </c>
-      <c r="I4" s="6">
-        <v>6</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="10">
         <v>0.46875</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="10">
         <v>0.53125</v>
       </c>
-      <c r="M4" t="s">
-        <v>78</v>
+      <c r="M4" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="O4" s="1"/>
     </row>
@@ -1162,12 +1194,6 @@
       <c r="G5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>16</v>
-      </c>
       <c r="J5" t="s">
         <v>17</v>
       </c>
@@ -1177,8 +1203,8 @@
       <c r="L5" s="2">
         <v>0.53125</v>
       </c>
-      <c r="M5" t="s">
-        <v>77</v>
+      <c r="M5" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="O5" s="1"/>
     </row>
@@ -1204,12 +1230,6 @@
       <c r="G6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>16</v>
-      </c>
       <c r="J6" t="s">
         <v>17</v>
       </c>
@@ -1218,6 +1238,9 @@
       </c>
       <c r="L6" s="2">
         <v>0.46875</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="O6" s="1"/>
     </row>
@@ -1243,12 +1266,6 @@
       <c r="G7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>16</v>
-      </c>
       <c r="J7" t="s">
         <v>15</v>
       </c>
@@ -1258,8 +1275,8 @@
       <c r="L7" s="2">
         <v>0.53125</v>
       </c>
-      <c r="M7" t="s">
-        <v>77</v>
+      <c r="M7" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="O7" s="1"/>
     </row>
@@ -1285,12 +1302,6 @@
       <c r="G8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H8">
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <v>16</v>
-      </c>
       <c r="J8" t="s">
         <v>11</v>
       </c>
@@ -1299,6 +1310,9 @@
       </c>
       <c r="L8" s="2">
         <v>0.71875</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="O8" s="1"/>
     </row>
@@ -1324,12 +1338,6 @@
       <c r="G9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H9">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <v>16</v>
-      </c>
       <c r="J9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1339,461 +1347,426 @@
       <c r="L9" s="2">
         <v>0.78125</v>
       </c>
-      <c r="M9" t="s">
-        <v>77</v>
+      <c r="M9" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="6">
-        <v>6</v>
-      </c>
-      <c r="I10" s="6">
-        <v>6</v>
-      </c>
-      <c r="J10" s="6" t="s">
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="10">
         <v>0.75</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="10">
         <v>0.8125</v>
       </c>
-      <c r="M10" t="s">
-        <v>78</v>
+      <c r="M10" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="C11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H11">
-        <v>6</v>
-      </c>
-      <c r="I11">
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0.4375</v>
+      </c>
+      <c r="L14" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0.46875</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0.53125</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0.65625</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0.71875</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K19" s="10">
+        <v>0.71875</v>
+      </c>
+      <c r="L19" s="10">
+        <v>0.78125</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J11" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="L11" s="2">
+      <c r="K20" s="10">
         <v>0.75</v>
       </c>
-      <c r="M11" t="s">
-        <v>77</v>
-      </c>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12">
-        <v>6</v>
-      </c>
-      <c r="I12">
-        <v>16</v>
-      </c>
-      <c r="J12" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13">
-        <v>6</v>
-      </c>
-      <c r="I13">
-        <v>16</v>
-      </c>
-      <c r="J13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0.6875</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="M13" t="s">
-        <v>77</v>
-      </c>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14">
-        <v>6</v>
-      </c>
-      <c r="I14">
-        <v>16</v>
-      </c>
-      <c r="J14" t="s">
-        <v>13</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0.4375</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15">
-        <v>6</v>
-      </c>
-      <c r="I15">
-        <v>16</v>
-      </c>
-      <c r="J15" t="s">
-        <v>13</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="L15" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="M15" t="s">
-        <v>77</v>
-      </c>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="6">
-        <v>6</v>
-      </c>
-      <c r="I16" s="6">
-        <v>6</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K16" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="L16" s="8">
-        <v>0.5625</v>
-      </c>
-      <c r="M16" t="s">
-        <v>78</v>
-      </c>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17">
-        <v>6</v>
-      </c>
-      <c r="I17">
-        <v>16</v>
-      </c>
-      <c r="J17" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0.46875</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0.53125</v>
-      </c>
-      <c r="M17" t="s">
-        <v>77</v>
-      </c>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18">
-        <v>6</v>
-      </c>
-      <c r="I18">
-        <v>16</v>
-      </c>
-      <c r="J18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K18" s="2">
-        <v>0.65625</v>
-      </c>
-      <c r="L18" s="2">
-        <v>0.71875</v>
-      </c>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19">
-        <v>6</v>
-      </c>
-      <c r="I19">
-        <v>16</v>
-      </c>
-      <c r="J19" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0.71875</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0.78125</v>
-      </c>
-      <c r="M19" t="s">
-        <v>77</v>
-      </c>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="6">
-        <v>6</v>
-      </c>
-      <c r="I20" s="6">
-        <v>6</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K20" s="8">
-        <v>0.75</v>
-      </c>
-      <c r="L20" s="8">
+      <c r="L20" s="10">
         <v>0.8125</v>
       </c>
-      <c r="M20" t="s">
-        <v>78</v>
+      <c r="M20" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="O20" s="1"/>
     </row>
@@ -1819,12 +1792,6 @@
       <c r="G21" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H21">
-        <v>6</v>
-      </c>
-      <c r="I21">
-        <v>16</v>
-      </c>
       <c r="J21" t="s">
         <v>12</v>
       </c>
@@ -1834,71 +1801,87 @@
       <c r="L21" s="2">
         <v>0.75</v>
       </c>
-      <c r="M21" t="s">
-        <v>77</v>
+      <c r="M21" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="O21" s="1"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
       </c>
-      <c r="E22" t="s">
-        <v>67</v>
+      <c r="E22">
+        <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="M22" t="s">
-        <v>75</v>
-      </c>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G22" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0.53125</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
       </c>
-      <c r="E23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M23" t="s">
-        <v>75</v>
-      </c>
-      <c r="O23" s="1"/>
+      <c r="E23">
+        <v>21</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0.46875</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.53125</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
@@ -1906,26 +1889,34 @@
       <c r="D24" t="s">
         <v>28</v>
       </c>
-      <c r="E24" t="s">
-        <v>72</v>
+      <c r="E24">
+        <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="M24" t="s">
-        <v>76</v>
-      </c>
-      <c r="O24" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>84</v>
+      </c>
+      <c r="J24" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
@@ -1933,19 +1924,227 @@
       <c r="D25" t="s">
         <v>31</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" t="s">
+        <v>85</v>
+      </c>
+      <c r="J25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26">
+        <v>15</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>16</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27">
+        <v>21</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>16</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N28" t="s">
+        <v>75</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N29" t="s">
+        <v>75</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
         <v>72</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F30" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G30" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.78125</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="M25" t="s">
+      <c r="J31" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N31" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="O25" s="1"/>
+      <c r="O31" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1969,13 +2168,13 @@
     <hyperlink ref="G19" r:id="rId18" xr:uid="{9422FABF-58D6-436F-A0C1-C9500E917A06}"/>
     <hyperlink ref="G20" r:id="rId19" xr:uid="{B2DD25FE-DBFC-4ECF-8716-83946099C0AC}"/>
     <hyperlink ref="G21" r:id="rId20" xr:uid="{FC746BE8-4CCF-4C04-B6F8-CF1C3E425C42}"/>
-    <hyperlink ref="G22" r:id="rId21" xr:uid="{EFC727B0-6EC5-4F35-80C3-BD00E20DAC5F}"/>
-    <hyperlink ref="G23" r:id="rId22" xr:uid="{77BA53EB-B704-454D-BC5F-46B0A390DCB2}"/>
-    <hyperlink ref="G24" r:id="rId23" xr:uid="{12B9DB10-F382-470E-A600-7CB708019B00}"/>
-    <hyperlink ref="G25" r:id="rId24" xr:uid="{B7FFE7F5-FAE0-4A70-8A8D-89C6CE0025BD}"/>
+    <hyperlink ref="G28" r:id="rId21" xr:uid="{EFC727B0-6EC5-4F35-80C3-BD00E20DAC5F}"/>
+    <hyperlink ref="G29" r:id="rId22" xr:uid="{77BA53EB-B704-454D-BC5F-46B0A390DCB2}"/>
+    <hyperlink ref="G30" r:id="rId23" xr:uid="{12B9DB10-F382-470E-A600-7CB708019B00}"/>
+    <hyperlink ref="G31" r:id="rId24" xr:uid="{B7FFE7F5-FAE0-4A70-8A8D-89C6CE0025BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>